<commit_message>
refine upsert built template stores
</commit_message>
<xml_diff>
--- a/apps/pczone/test/support/data/built_template_stores_shopee.xlsx
+++ b/apps/pczone/test/support/data/built_template_stores_shopee.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achilles/Projects/pczone_umbrella/apps/pczone/test/support/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D77FA58-BA63-A44E-BEAA-3A1B59EADBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D392753-ED4B-CE4B-823D-8FA00BDCD6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{B9F052DF-C490-8349-8AB1-D6D1286E076A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Máy tính mini PC HP EliteDesk 800 G2 65W core i5 6500</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>built_template_code</t>
+  </si>
+  <si>
+    <t>store_code</t>
+  </si>
+  <si>
+    <t>shopee</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE956FD3-2267-6649-BB00-29C9EC74C1BB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,7 +469,7 @@
     <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -473,8 +479,11 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -484,8 +493,11 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -495,8 +507,11 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -504,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -512,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -520,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -528,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -537,7 +552,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C8" xr:uid="{884A6457-F455-784B-8F62-EEC876248B81}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>